<commit_message>
changed data, the graph names were wrong
</commit_message>
<xml_diff>
--- a/progAssign2/CBC DATA.docx.xlsx
+++ b/progAssign2/CBC DATA.docx.xlsx
@@ -178,7 +178,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>DES 64bit Key (CTR)</a:t>
+              <a:t>DES 64bit Key (CBC)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -279,11 +279,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1068087864"/>
-        <c:axId val="74190183"/>
+        <c:axId val="1402746569"/>
+        <c:axId val="1708347332"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1068087864"/>
+        <c:axId val="1402746569"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -335,10 +335,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74190183"/>
+        <c:crossAx val="1708347332"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74190183"/>
+        <c:axId val="1708347332"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -413,7 +413,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1068087864"/>
+        <c:crossAx val="1402746569"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -463,7 +463,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>AES 128bit Key (CTR)</a:t>
+              <a:t>AES 128bit Key (CBC)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -564,11 +564,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1680298293"/>
-        <c:axId val="362376961"/>
+        <c:axId val="1987148939"/>
+        <c:axId val="1469013507"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1680298293"/>
+        <c:axId val="1987148939"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -620,10 +620,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362376961"/>
+        <c:crossAx val="1469013507"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362376961"/>
+        <c:axId val="1469013507"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,7 +698,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1680298293"/>
+        <c:crossAx val="1987148939"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -748,7 +748,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>3DES 64bit Key (CTR)</a:t>
+              <a:t>3DES 64bit Key (CBC)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -849,11 +849,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1997133031"/>
-        <c:axId val="314704383"/>
+        <c:axId val="363462129"/>
+        <c:axId val="81719581"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1997133031"/>
+        <c:axId val="363462129"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -905,10 +905,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314704383"/>
+        <c:crossAx val="81719581"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="314704383"/>
+        <c:axId val="81719581"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +983,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1997133031"/>
+        <c:crossAx val="363462129"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1033,7 +1033,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>AES 128bit Key (CTR)(HL)</a:t>
+              <a:t>AES 128bit Key (CBC)(HL)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1134,11 +1134,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1501289037"/>
-        <c:axId val="650971877"/>
+        <c:axId val="550168517"/>
+        <c:axId val="1879256505"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1501289037"/>
+        <c:axId val="550168517"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,10 +1190,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="650971877"/>
+        <c:crossAx val="1879256505"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="650971877"/>
+        <c:axId val="1879256505"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1268,7 +1268,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1501289037"/>
+        <c:crossAx val="550168517"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1318,7 +1318,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>AES 192bit Key (CTR)(HL)</a:t>
+              <a:t>AES 192bit Key (CBC)(HL)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1419,11 +1419,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="259877288"/>
-        <c:axId val="1821073667"/>
+        <c:axId val="1047078746"/>
+        <c:axId val="1243349351"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="259877288"/>
+        <c:axId val="1047078746"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,10 +1475,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1821073667"/>
+        <c:crossAx val="1243349351"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1821073667"/>
+        <c:axId val="1243349351"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1553,7 +1553,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259877288"/>
+        <c:crossAx val="1047078746"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1603,7 +1603,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>AES 256bit Key (CTR)(HL)</a:t>
+              <a:t>AES 256bit Key (CBC(HL)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1704,11 +1704,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1347384228"/>
-        <c:axId val="333181339"/>
+        <c:axId val="918814683"/>
+        <c:axId val="1149429815"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1347384228"/>
+        <c:axId val="918814683"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1760,10 +1760,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333181339"/>
+        <c:crossAx val="1149429815"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="333181339"/>
+        <c:axId val="1149429815"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1838,7 +1838,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1347384228"/>
+        <c:crossAx val="918814683"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1888,7 +1888,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>DES 64bit Key (CTR)(HL)</a:t>
+              <a:t>DES 64bit Key (CBC)(HL)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1989,11 +1989,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1245529885"/>
-        <c:axId val="977900674"/>
+        <c:axId val="1029226922"/>
+        <c:axId val="2094525053"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1245529885"/>
+        <c:axId val="1029226922"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2045,10 +2045,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="977900674"/>
+        <c:crossAx val="2094525053"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="977900674"/>
+        <c:axId val="2094525053"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2123,7 +2123,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1245529885"/>
+        <c:crossAx val="1029226922"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2173,7 +2173,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>3DES 64bit Key (CTR)(HL)</a:t>
+              <a:t>3DES 64bit Key (CBC)(HL)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2274,11 +2274,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2131105807"/>
-        <c:axId val="1130709993"/>
+        <c:axId val="1945534074"/>
+        <c:axId val="2115839348"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2131105807"/>
+        <c:axId val="1945534074"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2330,10 +2330,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1130709993"/>
+        <c:crossAx val="2115839348"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1130709993"/>
+        <c:axId val="2115839348"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2408,7 +2408,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131105807"/>
+        <c:crossAx val="1945534074"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2458,7 +2458,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>AES 256bit Key (CTR)</a:t>
+              <a:t>AES 256bit Key (CBC)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2559,11 +2559,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1680426923"/>
-        <c:axId val="1024015353"/>
+        <c:axId val="1631814816"/>
+        <c:axId val="1502828447"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1680426923"/>
+        <c:axId val="1631814816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2615,10 +2615,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1024015353"/>
+        <c:crossAx val="1502828447"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1024015353"/>
+        <c:axId val="1502828447"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2693,7 +2693,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1680426923"/>
+        <c:crossAx val="1631814816"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2743,7 +2743,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>AES 192bit Key (CTR)</a:t>
+              <a:t>AES 192bit Key (CBC)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2844,11 +2844,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1540258944"/>
-        <c:axId val="1695850069"/>
+        <c:axId val="1249317384"/>
+        <c:axId val="1544722701"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1540258944"/>
+        <c:axId val="1249317384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2900,10 +2900,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1695850069"/>
+        <c:crossAx val="1544722701"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1695850069"/>
+        <c:axId val="1544722701"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2978,7 +2978,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1540258944"/>
+        <c:crossAx val="1249317384"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>